<commit_message>
CP02PMUI D7 integration data and Cal sheet
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP02PMUI_00007.xlsx
+++ b/deployment/Omaha_Cal_Info_CP02PMUI_00007.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="2520" windowWidth="27120" windowHeight="16540" tabRatio="377"/>
+    <workbookView xWindow="4380" yWindow="2520" windowWidth="27120" windowHeight="16545" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$97</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$406</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="68">
   <si>
     <t>Ref Des</t>
   </si>
@@ -213,7 +218,37 @@
     <t>SWE 0007 Rev G</t>
   </si>
   <si>
-    <t>TBD</t>
+    <t>OL000243</t>
+  </si>
+  <si>
+    <t>OL000244</t>
+  </si>
+  <si>
+    <t>CP02PMUI-00007-MOPAK</t>
+  </si>
+  <si>
+    <t>OL000245</t>
+  </si>
+  <si>
+    <t>A00492</t>
+  </si>
+  <si>
+    <t>A00847</t>
+  </si>
+  <si>
+    <t>N00086</t>
+  </si>
+  <si>
+    <t>N00085</t>
+  </si>
+  <si>
+    <t>N00090</t>
+  </si>
+  <si>
+    <t>N00087</t>
+  </si>
+  <si>
+    <t>N00089</t>
   </si>
 </sst>
 </file>
@@ -226,7 +261,7 @@
     <numFmt numFmtId="166" formatCode="0.000000000000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -287,6 +322,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -302,14 +338,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,12 +355,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,7 +460,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -469,7 +493,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -516,8 +539,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -941,26 +964,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="19.1640625" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" customWidth="1"/>
-    <col min="12" max="12" width="15.83203125" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="13.5" customWidth="1"/>
+    <col min="8" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28">
+    <row r="1" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>49</v>
       </c>
@@ -998,8 +1021,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="12"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
       <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
@@ -1032,7 +1057,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
@@ -1049,916 +1074,1047 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
+    <row r="1" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="17">
-        <v>7</v>
-      </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="18">
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="16">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="17">
         <v>20496</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="32">
+      <c r="H2" s="31">
         <v>71000</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="14" t="s">
+      <c r="J2" s="32"/>
+      <c r="P2" s="32"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="17">
-        <v>7</v>
-      </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="18">
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="16">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="17">
         <v>20496</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="32">
+      <c r="H3" s="31">
         <v>40.365333333333332</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="14" t="s">
+      <c r="J3" s="32"/>
+      <c r="P3" s="32"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="17">
-        <v>7</v>
-      </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="18">
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="16">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="17">
         <v>20496</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="31">
         <v>-70.780900000000003</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="14"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="J4" s="32"/>
+      <c r="P4" s="32"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="14" t="s">
+      <c r="J5" s="32"/>
+      <c r="P5" s="32"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="17">
-        <v>7</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="16">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="16"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="14" t="s">
+      <c r="J6" s="32"/>
+      <c r="P6" s="32"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="22"/>
+      <c r="J7" s="32"/>
+      <c r="P7" s="32"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="17">
-        <v>7</v>
-      </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="18" t="s">
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="16">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="23">
         <v>-794.22</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="14" t="s">
+      <c r="J8" s="32"/>
+      <c r="P8" s="32"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="17">
-        <v>7</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="18" t="s">
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="16">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="31">
         <v>40.365333333333332</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="14" t="s">
+      <c r="J9" s="32"/>
+      <c r="P9" s="32"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="17">
-        <v>7</v>
-      </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="18" t="s">
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="16">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="31">
         <v>-70.780900000000003</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="14" t="s">
+      <c r="J10" s="32"/>
+      <c r="P10" s="32"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="17">
-        <v>7</v>
-      </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="18" t="s">
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="16">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="24">
         <v>2.6279E-4</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="14" t="s">
+      <c r="J11" s="32"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="17">
-        <v>7</v>
-      </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="18" t="s">
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="16">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="25">
         <v>-3.3176999999999998E-3</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="14" t="s">
+      <c r="J12" s="32"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="17">
-        <v>7</v>
-      </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="18" t="s">
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="16">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="24">
         <v>1.7828000000000001E-4</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="14" t="s">
+      <c r="J13" s="32"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="17">
-        <v>7</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="18" t="s">
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="16">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="26">
         <v>-2.3920000000000001E-6</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="14" t="s">
+      <c r="J14" s="32"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="17">
-        <v>7</v>
-      </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="18" t="s">
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="16">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="27">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="14"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="28"/>
+      <c r="J15" s="32"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="27"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="14" t="s">
+      <c r="J16" s="32"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="17">
-        <v>7</v>
-      </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="18">
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="16">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="17">
         <v>125</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="31">
         <v>40.365333333333332</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="14" t="s">
+      <c r="J17" s="32"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="17">
-        <v>7</v>
-      </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="18">
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="16">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="17">
         <v>125</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="31">
         <v>-70.780900000000003</v>
       </c>
       <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="14"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="29"/>
+      <c r="J18" s="32"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="28"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="14" t="s">
+      <c r="J19" s="32"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="17">
-        <v>7</v>
-      </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="18">
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="16">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="17">
         <v>100037</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H20" s="31">
         <v>40.365333333333332</v>
       </c>
       <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="14" t="s">
+      <c r="J20" s="32"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="17">
-        <v>7</v>
-      </c>
-      <c r="E21" s="22"/>
-      <c r="F21" s="18">
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="16">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="17">
         <v>100037</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="31">
         <v>-70.780900000000003</v>
       </c>
       <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="14"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="J21" s="32"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="14" t="s">
+      <c r="J22" s="32"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="17">
-        <v>7</v>
-      </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="18">
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="16">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="17">
         <v>1119</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="14">
         <v>1.0760000000000001</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="14" t="s">
+      <c r="J23" s="32"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="17">
-        <v>7</v>
-      </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="18">
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="16">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="17">
         <v>1119</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H24" s="29">
+      <c r="H24" s="28">
         <v>47</v>
       </c>
       <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="14" t="s">
+      <c r="J24" s="32"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="17">
-        <v>7</v>
-      </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="18">
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="16">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="17">
         <v>1119</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="29">
+      <c r="H25" s="28">
         <v>49</v>
       </c>
       <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="14" t="s">
+      <c r="J25" s="32"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="17">
-        <v>7</v>
-      </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="18">
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="16">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="17">
         <v>1119</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="29">
+      <c r="H26" s="28">
         <v>48</v>
       </c>
       <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="14" t="s">
+      <c r="J26" s="32"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="17">
-        <v>7</v>
-      </c>
-      <c r="E27" s="22"/>
-      <c r="F27" s="18">
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="16">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="17">
         <v>1119</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="14">
         <v>3.9E-2</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="14" t="s">
+      <c r="J27" s="32"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="17">
-        <v>7</v>
-      </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="18">
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="16">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="17">
         <v>1119</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="14">
         <v>700</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="14" t="s">
+      <c r="J28" s="32"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="17">
-        <v>7</v>
-      </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="18">
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="16">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="17">
         <v>1119</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H29" s="29">
+      <c r="H29" s="28">
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="14" t="s">
+      <c r="J29" s="32"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="17">
-        <v>7</v>
-      </c>
-      <c r="E30" s="22"/>
-      <c r="F30" s="18">
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="16">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="17">
         <v>1119</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H30" s="29">
+      <c r="H30" s="28">
         <v>1.14E-2</v>
       </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="14" t="s">
+      <c r="J30" s="32"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="17">
-        <v>7</v>
-      </c>
-      <c r="E31" s="22"/>
-      <c r="F31" s="18">
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="16">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="17">
         <v>1119</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H31" s="30">
+      <c r="H31" s="29">
         <v>3.0690000000000002E-6</v>
       </c>
       <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="14" t="s">
+      <c r="J31" s="32"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="17">
-        <v>7</v>
-      </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="18">
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="16">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="17">
         <v>1119</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="14">
         <v>124</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="14"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
+      <c r="J32" s="32"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="14" t="s">
+      <c r="J33" s="32"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="17">
-        <v>7</v>
-      </c>
-      <c r="E34" s="22"/>
-      <c r="F34" s="18">
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="16">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="17">
         <v>20465</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H34" s="29">
+      <c r="H34" s="28">
         <v>1.2</v>
       </c>
       <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="14" t="s">
+      <c r="J34" s="32"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="17">
-        <v>7</v>
-      </c>
-      <c r="E35" s="22"/>
-      <c r="F35" s="18">
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="16">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="17">
         <v>20465</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H35" s="30">
+      <c r="H35" s="29">
         <v>1.01E-17</v>
       </c>
       <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="14"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="29"/>
+      <c r="J35" s="32"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="28"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="14" t="s">
+      <c r="J36" s="32"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="17">
-        <v>7</v>
-      </c>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22" t="s">
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="16">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
       <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="16"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="14" t="s">
+      <c r="J37" s="32"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="J38" s="32"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D39" s="17">
-        <v>7</v>
-      </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="31" t="s">
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="16">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="14"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
+      <c r="J39" s="32"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="16"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="J40" s="32"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E48" s="2"/>
     </row>
   </sheetData>

</xml_diff>